<commit_message>
* ALU test bench
</commit_message>
<xml_diff>
--- a/dessins/Control.xlsx
+++ b/dessins/Control.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4505"/>
   <workbookPr checkCompatibility="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="4120" yWindow="1740" windowWidth="35040" windowHeight="17440"/>
+    <workbookView xWindow="3760" yWindow="-420" windowWidth="35320" windowHeight="23300"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="79">
   <si>
     <t xml:space="preserve">Instr </t>
   </si>
@@ -307,6 +307,38 @@
   </si>
   <si>
     <t>00</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AluOp</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>XXX</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>001</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>111</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>010</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>011</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -353,7 +385,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="20">
     <border>
       <left/>
       <right/>
@@ -478,11 +510,115 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -521,6 +657,30 @@
     <xf numFmtId="49" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -542,13 +702,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>3</xdr:col>
+      <xdr:col>4</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>200526</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
+      <xdr:col>5</xdr:col>
       <xdr:colOff>73162</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>200526</xdr:rowOff>
@@ -558,7 +718,7 @@
         <xdr:cNvPr id="2" name="Picture 1" descr="page5image5010080">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D1065E6A-2946-EB49-85D5-532CB59FAFF5}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns="" id="{D1065E6A-2946-EB49-85D5-532CB59FAFF5}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -570,7 +730,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns="" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns="" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -590,7 +750,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns="" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns="">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -603,13 +763,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>4</xdr:col>
+      <xdr:col>5</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>200526</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
+      <xdr:col>5</xdr:col>
       <xdr:colOff>533400</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>200526</xdr:rowOff>
@@ -619,7 +779,7 @@
         <xdr:cNvPr id="3" name="Picture 2" descr="page5image5013216">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6B7E070A-7D7D-5E41-A85A-297765A2C47F}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns="" id="{6B7E070A-7D7D-5E41-A85A-297765A2C47F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -631,7 +791,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns="" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns="" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -651,129 +811,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns="" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>73162</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Picture 3" descr="page5image5027440">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E0BD7523-80DB-9D45-AC23-60E152D26724}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns="" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="1651000" y="1638300"/>
-          <a:ext cx="711200" cy="0"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns="" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>73162</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="5" name="Picture 4" descr="page5image5027664">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3F8DAB48-D435-0543-9727-709FD51CD5FC}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns="" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="1651000" y="2463800"/>
-          <a:ext cx="711200" cy="0"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns="" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns="">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -792,17 +830,17 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>533400</xdr:colOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>73162</xdr:colOff>
       <xdr:row>3</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="6" name="Picture 5" descr="page5image5027776">
+        <xdr:cNvPr id="4" name="Picture 3" descr="page5image5027440">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0E82F135-FC04-7E46-A379-6AE6C1F1F79A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns="" id="{E0BD7523-80DB-9D45-AC23-60E152D26724}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -811,10 +849,10 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns="" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns="" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -825,8 +863,8 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="2476500" y="1638300"/>
-          <a:ext cx="533400" cy="0"/>
+          <a:off x="1651000" y="1638300"/>
+          <a:ext cx="711200" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -834,7 +872,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns="" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns="">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -853,7 +891,129 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>73162</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4" descr="page5image5027664">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns="" id="{3F8DAB48-D435-0543-9727-709FD51CD5FC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns="" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="1651000" y="2463800"/>
+          <a:ext cx="711200" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns="">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>533400</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5" descr="page5image5027776">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns="" id="{0E82F135-FC04-7E46-A379-6AE6C1F1F79A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns="" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="2476500" y="1638300"/>
+          <a:ext cx="533400" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns="">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
       <xdr:colOff>533400</xdr:colOff>
       <xdr:row>4</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -863,7 +1023,7 @@
         <xdr:cNvPr id="7" name="Picture 6" descr="page5image5051744">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C97A34F3-001F-0F44-9233-FDA963BA405C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns="" id="{C97A34F3-001F-0F44-9233-FDA963BA405C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -875,7 +1035,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns="" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns="" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -895,7 +1055,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns="" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns="">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -924,7 +1084,7 @@
         <xdr:cNvPr id="8" name="Picture 7" descr="page5image2911024">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{63E28791-EFBD-CB48-8EE3-5E8D0268E1BA}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns="" id="{63E28791-EFBD-CB48-8EE3-5E8D0268E1BA}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -936,7 +1096,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns="" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns="" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -956,7 +1116,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns="" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns="">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -969,13 +1129,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>4</xdr:col>
+      <xdr:col>5</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>4</xdr:row>
       <xdr:rowOff>200526</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
+      <xdr:col>5</xdr:col>
       <xdr:colOff>533400</xdr:colOff>
       <xdr:row>4</xdr:row>
       <xdr:rowOff>200526</xdr:rowOff>
@@ -985,7 +1145,7 @@
         <xdr:cNvPr id="9" name="Picture 8" descr="page5image3004320">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{99CF0BA2-88C3-7942-84F9-F580B832725A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns="" id="{99CF0BA2-88C3-7942-84F9-F580B832725A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -997,7 +1157,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns="" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns="" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -1017,7 +1177,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns="" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns="">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -1030,13 +1190,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>6</xdr:col>
+      <xdr:col>7</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>6</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
+      <xdr:col>7</xdr:col>
       <xdr:colOff>12700</xdr:colOff>
       <xdr:row>6</xdr:row>
       <xdr:rowOff>12700</xdr:rowOff>
@@ -1046,7 +1206,7 @@
         <xdr:cNvPr id="10" name="Picture 9" descr="page5image3702672">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BCAE4D06-488E-484E-8B1C-88EBA259AEF7}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns="" id="{BCAE4D06-488E-484E-8B1C-88EBA259AEF7}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1058,7 +1218,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns="" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns="" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -1078,7 +1238,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns="" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns="">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -1091,13 +1251,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>6</xdr:col>
+      <xdr:col>7</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>9</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
+      <xdr:col>7</xdr:col>
       <xdr:colOff>12700</xdr:colOff>
       <xdr:row>9</xdr:row>
       <xdr:rowOff>12700</xdr:rowOff>
@@ -1107,7 +1267,7 @@
         <xdr:cNvPr id="11" name="Picture 10" descr="page5image3703712">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{34A007C2-32FF-F946-A78C-55C38D0F8D6A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns="" id="{34A007C2-32FF-F946-A78C-55C38D0F8D6A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1119,7 +1279,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns="" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns="" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -1139,7 +1299,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns="" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns="">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -1168,7 +1328,7 @@
         <xdr:cNvPr id="12" name="Picture 11" descr="page5image3705792">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A49356F5-0746-F04F-9A08-57C13038F148}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns="" id="{A49356F5-0746-F04F-9A08-57C13038F148}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1180,7 +1340,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns="" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns="" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -1200,7 +1360,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns="" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns="">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -1229,7 +1389,7 @@
         <xdr:cNvPr id="13" name="Picture 12" descr="page5image3706416">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D897A736-EA77-CA45-BE72-EBD7887E488E}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns="" id="{D897A736-EA77-CA45-BE72-EBD7887E488E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1241,7 +1401,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns="" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns="" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -1261,7 +1421,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns="" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns="">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -1290,7 +1450,7 @@
         <xdr:cNvPr id="14" name="Picture 13" descr="page5image3706832">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{336BB3DD-E9B5-F948-AB95-28F2AE85AA33}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns="" id="{336BB3DD-E9B5-F948-AB95-28F2AE85AA33}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1302,7 +1462,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns="" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns="" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -1322,7 +1482,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns="" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns="">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -1351,7 +1511,7 @@
         <xdr:cNvPr id="15" name="Picture 14" descr="page5image3707456">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0C0A9650-BBE9-1248-AFEA-7107D1E31E35}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns="" id="{0C0A9650-BBE9-1248-AFEA-7107D1E31E35}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1363,7 +1523,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns="" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns="" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -1383,7 +1543,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns="" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns="">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -1396,14 +1556,14 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>6</xdr:col>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>800100</xdr:colOff>
       <xdr:row>6</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>61678</xdr:colOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>62711</xdr:colOff>
       <xdr:row>6</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
@@ -1412,7 +1572,7 @@
         <xdr:cNvPr id="16" name="Picture 15" descr="page5image2911024">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{63E28791-EFBD-CB48-8EE3-5E8D0268E1BA}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns="" id="{63E28791-EFBD-CB48-8EE3-5E8D0268E1BA}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1424,7 +1584,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns="" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns="" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -1444,7 +1604,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns="" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns="">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -1457,13 +1617,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>7</xdr:col>
+      <xdr:col>3</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>6</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
+      <xdr:col>3</xdr:col>
       <xdr:colOff>12700</xdr:colOff>
       <xdr:row>6</xdr:row>
       <xdr:rowOff>12700</xdr:rowOff>
@@ -1473,7 +1633,7 @@
         <xdr:cNvPr id="17" name="Picture 16" descr="page5image3706832">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{336BB3DD-E9B5-F948-AB95-28F2AE85AA33}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns="" id="{336BB3DD-E9B5-F948-AB95-28F2AE85AA33}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1485,7 +1645,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns="" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns="" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -1505,7 +1665,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns="" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns="">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -1808,7 +1968,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1819,10 +1979,10 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:L16"/>
+  <dimension ref="A1:N16"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" zoomScale="209" zoomScaleNormal="209" zoomScalePageLayoutView="209" workbookViewId="0">
-      <selection activeCell="M3" sqref="M3"/>
+    <sheetView tabSelected="1" zoomScale="209" zoomScaleNormal="209" zoomScalePageLayoutView="209" workbookViewId="0">
+      <selection activeCell="M9" sqref="M9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1830,40 +1990,42 @@
     <col min="1" max="1" width="11.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="6.83203125" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="7" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.5" style="1" customWidth="1"/>
+    <col min="5" max="5" width="8.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="7" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="6.83203125" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="9.1640625" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="9.5" style="1" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="5.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="18" thickBot="1">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:14" ht="18" thickBot="1">
+      <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>47</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>42</v>
       </c>
       <c r="I1" s="3" t="s">
         <v>3</v>
@@ -1874,34 +2036,37 @@
       <c r="K1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="L1" s="3" t="s">
         <v>6</v>
       </c>
+      <c r="M1" s="18" t="s">
+        <v>71</v>
+      </c>
     </row>
-    <row r="2" spans="1:12" ht="16" customHeight="1">
-      <c r="A2" s="5" t="s">
+    <row r="2" spans="1:14" ht="16" customHeight="1">
+      <c r="A2" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="6">
+      <c r="D2" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="E2" s="6">
         <v>1</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="F2" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="G2" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="H2" s="6" t="s">
         <v>45</v>
-      </c>
-      <c r="H2" s="6" t="s">
-        <v>49</v>
       </c>
       <c r="I2" s="6">
         <v>0</v>
@@ -1912,34 +2077,41 @@
       <c r="K2" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="L2" s="7" t="s">
+      <c r="L2" s="6" t="s">
         <v>45</v>
       </c>
+      <c r="M2" s="19" t="s">
+        <v>76</v>
+      </c>
+      <c r="N2" s="9" t="str">
+        <f>CONCATENATE(E2,F2,G2,H2,I2,J2,K2,L2,M2)</f>
+        <v>101000000000111</v>
+      </c>
     </row>
-    <row r="3" spans="1:12" ht="16" customHeight="1">
-      <c r="A3" s="8" t="s">
+    <row r="3" spans="1:14" ht="16" customHeight="1">
+      <c r="A3" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="9">
+      <c r="B3" s="8">
         <v>100011</v>
       </c>
-      <c r="C3" s="9">
+      <c r="C3" s="10">
         <v>100000</v>
       </c>
-      <c r="D3" s="9">
+      <c r="D3" s="8">
+        <v>100000</v>
+      </c>
+      <c r="E3" s="9">
         <v>1</v>
       </c>
-      <c r="E3" s="9" t="s">
+      <c r="F3" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="F3" s="9" t="s">
+      <c r="G3" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="G3" s="9" t="s">
+      <c r="H3" s="9" t="s">
         <v>51</v>
-      </c>
-      <c r="H3" s="9">
-        <v>100000</v>
       </c>
       <c r="I3" s="9">
         <v>0</v>
@@ -1950,34 +2122,41 @@
       <c r="K3" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="L3" s="10" t="s">
+      <c r="L3" s="9" t="s">
         <v>45</v>
       </c>
+      <c r="M3" s="20" t="s">
+        <v>74</v>
+      </c>
+      <c r="N3" s="9" t="str">
+        <f t="shared" ref="N3:N16" si="0">CONCATENATE(E3,F3,G3,H3,I3,J3,K3,L3,M3)</f>
+        <v>100001000100000</v>
+      </c>
     </row>
-    <row r="4" spans="1:12" ht="16" customHeight="1">
-      <c r="A4" s="8" t="s">
+    <row r="4" spans="1:14" ht="16" customHeight="1">
+      <c r="A4" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="9">
+      <c r="B4" s="8">
         <v>101011</v>
       </c>
-      <c r="C4" s="9">
+      <c r="C4" s="10">
         <v>100000</v>
       </c>
-      <c r="D4" s="9">
+      <c r="D4" s="8">
+        <v>100000</v>
+      </c>
+      <c r="E4" s="9">
         <v>0</v>
       </c>
-      <c r="E4" s="9" t="s">
+      <c r="F4" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="F4" s="9" t="s">
+      <c r="G4" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="G4" s="9" t="s">
+      <c r="H4" s="9" t="s">
         <v>51</v>
-      </c>
-      <c r="H4" s="9">
-        <v>100000</v>
       </c>
       <c r="I4" s="9">
         <v>0</v>
@@ -1988,34 +2167,41 @@
       <c r="K4" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="L4" s="10" t="s">
+      <c r="L4" s="9" t="s">
         <v>45</v>
       </c>
+      <c r="M4" s="20" t="s">
+        <v>74</v>
+      </c>
+      <c r="N4" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>0XX00101XX00000</v>
+      </c>
     </row>
-    <row r="5" spans="1:12" ht="16" customHeight="1">
-      <c r="A5" s="8" t="s">
+    <row r="5" spans="1:14" ht="16" customHeight="1">
+      <c r="A5" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="9" t="s">
+      <c r="B5" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="9">
+      <c r="C5" s="10">
         <v>100010</v>
       </c>
-      <c r="D5" s="9">
+      <c r="D5" s="8">
+        <v>100010</v>
+      </c>
+      <c r="E5" s="9">
         <v>0</v>
       </c>
-      <c r="E5" s="9" t="s">
+      <c r="F5" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="F5" s="9" t="s">
+      <c r="G5" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="G5" s="9" t="s">
+      <c r="H5" s="9" t="s">
         <v>45</v>
-      </c>
-      <c r="H5" s="9">
-        <v>100010</v>
       </c>
       <c r="I5" s="9">
         <v>1</v>
@@ -2026,34 +2212,41 @@
       <c r="K5" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="L5" s="10" t="s">
+      <c r="L5" s="9" t="s">
         <v>45</v>
       </c>
+      <c r="M5" s="20" t="s">
+        <v>75</v>
+      </c>
+      <c r="N5" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>0XX00010XX00001</v>
+      </c>
     </row>
-    <row r="6" spans="1:12" ht="16" customHeight="1">
-      <c r="A6" s="8" t="s">
+    <row r="6" spans="1:14" ht="16" customHeight="1">
+      <c r="A6" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="9" t="s">
+      <c r="B6" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="9" t="s">
+      <c r="C6" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="D6" s="9">
+      <c r="D6" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="E6" s="9">
         <v>0</v>
       </c>
-      <c r="E6" s="9" t="s">
+      <c r="F6" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="F6" s="9" t="s">
+      <c r="G6" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="G6" s="9" t="s">
+      <c r="H6" s="9" t="s">
         <v>53</v>
-      </c>
-      <c r="H6" s="9" t="s">
-        <v>54</v>
       </c>
       <c r="I6" s="9" t="s">
         <v>19</v>
@@ -2064,34 +2257,41 @@
       <c r="K6" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="L6" s="10" t="s">
+      <c r="L6" s="9" t="s">
         <v>51</v>
       </c>
+      <c r="M6" s="20" t="s">
+        <v>74</v>
+      </c>
+      <c r="N6" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>0XXXXXX0XX01000</v>
+      </c>
     </row>
-    <row r="7" spans="1:12" ht="16" customHeight="1" thickBot="1">
-      <c r="A7" s="11" t="s">
+    <row r="7" spans="1:14" ht="16" customHeight="1" thickBot="1">
+      <c r="A7" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="12" t="s">
+      <c r="B7" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="12">
+      <c r="C7" s="13">
         <v>100000</v>
       </c>
-      <c r="D7" s="12">
+      <c r="D7" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="E7" s="12">
         <v>1</v>
       </c>
-      <c r="E7" s="12" t="s">
+      <c r="F7" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="F7" s="12" t="s">
+      <c r="G7" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="G7" s="12" t="s">
+      <c r="H7" s="12" t="s">
         <v>51</v>
-      </c>
-      <c r="H7" s="12" t="s">
-        <v>55</v>
       </c>
       <c r="I7" s="12">
         <v>0</v>
@@ -2102,72 +2302,86 @@
       <c r="K7" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="L7" s="13" t="s">
+      <c r="L7" s="12" t="s">
         <v>45</v>
       </c>
+      <c r="M7" s="21" t="s">
+        <v>74</v>
+      </c>
+      <c r="N7" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>100001000000000</v>
+      </c>
     </row>
-    <row r="8" spans="1:12" ht="16" customHeight="1">
-      <c r="A8" s="5" t="s">
+    <row r="8" spans="1:14" ht="16" customHeight="1">
+      <c r="A8" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="C8" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="D8" s="6" t="s">
+      <c r="D8" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="E8" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="E8" s="6" t="s">
+      <c r="F8" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="F8" s="6" t="s">
+      <c r="G8" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="G8" s="6" t="s">
+      <c r="H8" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="H8" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="I8" s="6" t="s">
+      <c r="I8" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="J8" s="6" t="s">
+      <c r="J8" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="K8" s="6" t="s">
+      <c r="K8" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="L8" s="7" t="s">
+      <c r="L8" s="9" t="s">
         <v>58</v>
       </c>
+      <c r="M8" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="N8" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>0XXXXXX0XX10111</v>
+      </c>
     </row>
-    <row r="9" spans="1:12" ht="16" customHeight="1">
-      <c r="A9" s="8" t="s">
+    <row r="9" spans="1:14" ht="16" customHeight="1">
+      <c r="A9" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="B9" s="9" t="s">
+      <c r="B9" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="C9" s="9" t="s">
+      <c r="C9" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="D9" s="9" t="s">
+      <c r="D9" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="E9" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="E9" s="9" t="s">
+      <c r="F9" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="F9" s="9" t="s">
+      <c r="G9" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="G9" s="9" t="s">
+      <c r="H9" s="9" t="s">
         <v>58</v>
-      </c>
-      <c r="H9" s="9" t="s">
-        <v>60</v>
       </c>
       <c r="I9" s="9" t="s">
         <v>48</v>
@@ -2178,34 +2392,41 @@
       <c r="K9" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="L9" s="10" t="s">
+      <c r="L9" s="9" t="s">
         <v>45</v>
       </c>
+      <c r="M9" s="20" t="s">
+        <v>77</v>
+      </c>
+      <c r="N9" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>100010000000010</v>
+      </c>
     </row>
-    <row r="10" spans="1:12" ht="16" customHeight="1">
-      <c r="A10" s="8" t="s">
+    <row r="10" spans="1:14" ht="16" customHeight="1">
+      <c r="A10" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="B10" s="9" t="s">
+      <c r="B10" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="C10" s="9" t="s">
+      <c r="C10" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="D10" s="9" t="s">
+      <c r="D10" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="E10" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="E10" s="9" t="s">
+      <c r="F10" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="F10" s="9" t="s">
+      <c r="G10" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="G10" s="9" t="s">
+      <c r="H10" s="9" t="s">
         <v>58</v>
-      </c>
-      <c r="H10" s="9" t="s">
-        <v>61</v>
       </c>
       <c r="I10" s="9" t="s">
         <v>48</v>
@@ -2216,34 +2437,41 @@
       <c r="K10" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="L10" s="10" t="s">
+      <c r="L10" s="9" t="s">
         <v>45</v>
       </c>
+      <c r="M10" s="20" t="s">
+        <v>78</v>
+      </c>
+      <c r="N10" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>100010000000011</v>
+      </c>
     </row>
-    <row r="11" spans="1:12" ht="16" customHeight="1">
-      <c r="A11" s="8" t="s">
+    <row r="11" spans="1:14" ht="16" customHeight="1">
+      <c r="A11" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="B11" s="9" t="s">
+      <c r="B11" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="C11" s="9" t="s">
+      <c r="C11" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="D11" s="9" t="s">
+      <c r="D11" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="E11" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="E11" s="9" t="s">
+      <c r="F11" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="F11" s="9" t="s">
+      <c r="G11" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="G11" s="9" t="s">
+      <c r="H11" s="9" t="s">
         <v>53</v>
-      </c>
-      <c r="H11" s="9" t="s">
-        <v>57</v>
       </c>
       <c r="I11" s="9" t="s">
         <v>19</v>
@@ -2254,34 +2482,41 @@
       <c r="K11" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="L11" s="10" t="s">
+      <c r="L11" s="9" t="s">
         <v>51</v>
       </c>
+      <c r="M11" s="20" t="s">
+        <v>72</v>
+      </c>
+      <c r="N11" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>110XXXX01101XXX</v>
+      </c>
     </row>
-    <row r="12" spans="1:12" ht="16" customHeight="1">
-      <c r="A12" s="8" t="s">
+    <row r="12" spans="1:14" ht="16" customHeight="1">
+      <c r="A12" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="B12" s="9" t="s">
+      <c r="B12" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="C12" s="9" t="s">
+      <c r="C12" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="D12" s="9" t="s">
+      <c r="D12" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="E12" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="E12" s="9" t="s">
+      <c r="F12" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="F12" s="9" t="s">
+      <c r="G12" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="G12" s="9" t="s">
+      <c r="H12" s="9" t="s">
         <v>53</v>
-      </c>
-      <c r="H12" s="9" t="s">
-        <v>57</v>
       </c>
       <c r="I12" s="9" t="s">
         <v>48</v>
@@ -2292,34 +2527,41 @@
       <c r="K12" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="L12" s="10" t="s">
+      <c r="L12" s="9" t="s">
         <v>45</v>
       </c>
+      <c r="M12" s="20" t="s">
+        <v>72</v>
+      </c>
+      <c r="N12" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>100XXX001000XXX</v>
+      </c>
     </row>
-    <row r="13" spans="1:12">
-      <c r="A13" s="8" t="s">
+    <row r="13" spans="1:14">
+      <c r="A13" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="B13" s="9" t="s">
+      <c r="B13" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C13" s="9" t="s">
+      <c r="C13" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="D13" s="9" t="s">
+      <c r="D13" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="E13" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="E13" s="9" t="s">
+      <c r="F13" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="F13" s="9" t="s">
+      <c r="G13" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="G13" s="9" t="s">
+      <c r="H13" s="9" t="s">
         <v>45</v>
-      </c>
-      <c r="H13" s="9" t="s">
-        <v>14</v>
       </c>
       <c r="I13" s="9" t="s">
         <v>18</v>
@@ -2330,34 +2572,41 @@
       <c r="K13" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="L13" s="10" t="s">
+      <c r="L13" s="9" t="s">
         <v>63</v>
       </c>
+      <c r="M13" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="N13" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>101X00000000111</v>
+      </c>
     </row>
-    <row r="14" spans="1:12">
-      <c r="A14" s="8" t="s">
+    <row r="14" spans="1:14">
+      <c r="A14" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="B14" s="9" t="s">
+      <c r="B14" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C14" s="9" t="s">
+      <c r="C14" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="D14" s="9" t="s">
+      <c r="D14" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="E14" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="E14" s="9" t="s">
+      <c r="F14" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="F14" s="9" t="s">
+      <c r="G14" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="G14" s="9" t="s">
+      <c r="H14" s="9" t="s">
         <v>70</v>
-      </c>
-      <c r="H14" s="9" t="s">
-        <v>65</v>
       </c>
       <c r="I14" s="9" t="s">
         <v>18</v>
@@ -2368,34 +2617,41 @@
       <c r="K14" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="L14" s="10" t="s">
+      <c r="L14" s="9" t="s">
         <v>45</v>
       </c>
+      <c r="M14" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="N14" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>101000000000111</v>
+      </c>
     </row>
-    <row r="15" spans="1:12">
-      <c r="A15" s="8" t="s">
+    <row r="15" spans="1:14">
+      <c r="A15" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="B15" s="9" t="s">
+      <c r="B15" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C15" s="9" t="s">
+      <c r="C15" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="D15" s="9" t="s">
+      <c r="D15" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="E15" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="E15" s="9" t="s">
+      <c r="F15" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="F15" s="9" t="s">
+      <c r="G15" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="G15" s="9" t="s">
+      <c r="H15" s="9" t="s">
         <v>70</v>
-      </c>
-      <c r="H15" s="9" t="s">
-        <v>66</v>
       </c>
       <c r="I15" s="9" t="s">
         <v>18</v>
@@ -2406,34 +2662,41 @@
       <c r="K15" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="L15" s="10" t="s">
+      <c r="L15" s="9" t="s">
         <v>45</v>
       </c>
+      <c r="M15" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="N15" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>101000000000111</v>
+      </c>
     </row>
-    <row r="16" spans="1:12" ht="16" thickBot="1">
-      <c r="A16" s="11" t="s">
+    <row r="16" spans="1:14" ht="16" thickBot="1">
+      <c r="A16" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="B16" s="12" t="s">
+      <c r="B16" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="C16" s="12" t="s">
+      <c r="C16" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="D16" s="12" t="s">
+      <c r="D16" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="E16" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="E16" s="12" t="s">
+      <c r="F16" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="F16" s="12" t="s">
+      <c r="G16" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="G16" s="12" t="s">
+      <c r="H16" s="12" t="s">
         <v>45</v>
-      </c>
-      <c r="H16" s="12" t="s">
-        <v>55</v>
       </c>
       <c r="I16" s="12" t="s">
         <v>43</v>
@@ -2444,8 +2707,15 @@
       <c r="K16" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="L16" s="13" t="s">
+      <c r="L16" s="12" t="s">
         <v>45</v>
+      </c>
+      <c r="M16" s="21" t="s">
+        <v>73</v>
+      </c>
+      <c r="N16" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>101100000000000</v>
       </c>
     </row>
   </sheetData>
@@ -2455,7 +2725,7 @@
   <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
-      <mx:PLV Mode="1" OnePage="0" WScale="0"/>
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
     </ext>
   </extLst>
 </worksheet>

</xml_diff>

<commit_message>
* control file update
</commit_message>
<xml_diff>
--- a/dessins/Control.xlsx
+++ b/dessins/Control.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4505"/>
   <workbookPr checkCompatibility="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="4120" yWindow="1740" windowWidth="35040" windowHeight="17440"/>
+    <workbookView xWindow="3760" yWindow="-420" windowWidth="35320" windowHeight="23300"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="79">
   <si>
     <t xml:space="preserve">Instr </t>
   </si>
@@ -307,6 +307,38 @@
   </si>
   <si>
     <t>00</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AluOp</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>XXX</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>001</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>111</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>010</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>011</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -353,7 +385,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="20">
     <border>
       <left/>
       <right/>
@@ -478,11 +510,115 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -521,6 +657,30 @@
     <xf numFmtId="49" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -542,13 +702,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>3</xdr:col>
+      <xdr:col>4</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>200526</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
+      <xdr:col>5</xdr:col>
       <xdr:colOff>73162</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>200526</xdr:rowOff>
@@ -558,7 +718,7 @@
         <xdr:cNvPr id="2" name="Picture 1" descr="page5image5010080">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D1065E6A-2946-EB49-85D5-532CB59FAFF5}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns="" id="{D1065E6A-2946-EB49-85D5-532CB59FAFF5}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -570,7 +730,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns="" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns="" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -590,7 +750,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns="" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns="">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -603,13 +763,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>4</xdr:col>
+      <xdr:col>5</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>200526</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
+      <xdr:col>5</xdr:col>
       <xdr:colOff>533400</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>200526</xdr:rowOff>
@@ -619,7 +779,7 @@
         <xdr:cNvPr id="3" name="Picture 2" descr="page5image5013216">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6B7E070A-7D7D-5E41-A85A-297765A2C47F}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns="" id="{6B7E070A-7D7D-5E41-A85A-297765A2C47F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -631,7 +791,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns="" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns="" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -651,129 +811,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns="" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>73162</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Picture 3" descr="page5image5027440">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E0BD7523-80DB-9D45-AC23-60E152D26724}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns="" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="1651000" y="1638300"/>
-          <a:ext cx="711200" cy="0"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns="" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>73162</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="5" name="Picture 4" descr="page5image5027664">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3F8DAB48-D435-0543-9727-709FD51CD5FC}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns="" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="1651000" y="2463800"/>
-          <a:ext cx="711200" cy="0"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns="" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns="">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -792,17 +830,17 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>533400</xdr:colOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>73162</xdr:colOff>
       <xdr:row>3</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="6" name="Picture 5" descr="page5image5027776">
+        <xdr:cNvPr id="4" name="Picture 3" descr="page5image5027440">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0E82F135-FC04-7E46-A379-6AE6C1F1F79A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns="" id="{E0BD7523-80DB-9D45-AC23-60E152D26724}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -811,10 +849,10 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns="" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns="" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -825,8 +863,8 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="2476500" y="1638300"/>
-          <a:ext cx="533400" cy="0"/>
+          <a:off x="1651000" y="1638300"/>
+          <a:ext cx="711200" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -834,7 +872,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns="" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns="">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -853,7 +891,129 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>73162</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4" descr="page5image5027664">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns="" id="{3F8DAB48-D435-0543-9727-709FD51CD5FC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns="" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="1651000" y="2463800"/>
+          <a:ext cx="711200" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns="">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>533400</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5" descr="page5image5027776">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns="" id="{0E82F135-FC04-7E46-A379-6AE6C1F1F79A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns="" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="2476500" y="1638300"/>
+          <a:ext cx="533400" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns="">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
       <xdr:colOff>533400</xdr:colOff>
       <xdr:row>4</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -863,7 +1023,7 @@
         <xdr:cNvPr id="7" name="Picture 6" descr="page5image5051744">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C97A34F3-001F-0F44-9233-FDA963BA405C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns="" id="{C97A34F3-001F-0F44-9233-FDA963BA405C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -875,7 +1035,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns="" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns="" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -895,7 +1055,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns="" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns="">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -924,7 +1084,7 @@
         <xdr:cNvPr id="8" name="Picture 7" descr="page5image2911024">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{63E28791-EFBD-CB48-8EE3-5E8D0268E1BA}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns="" id="{63E28791-EFBD-CB48-8EE3-5E8D0268E1BA}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -936,7 +1096,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns="" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns="" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -956,7 +1116,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns="" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns="">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -969,13 +1129,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>4</xdr:col>
+      <xdr:col>5</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>4</xdr:row>
       <xdr:rowOff>200526</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
+      <xdr:col>5</xdr:col>
       <xdr:colOff>533400</xdr:colOff>
       <xdr:row>4</xdr:row>
       <xdr:rowOff>200526</xdr:rowOff>
@@ -985,7 +1145,7 @@
         <xdr:cNvPr id="9" name="Picture 8" descr="page5image3004320">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{99CF0BA2-88C3-7942-84F9-F580B832725A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns="" id="{99CF0BA2-88C3-7942-84F9-F580B832725A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -997,7 +1157,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns="" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns="" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -1017,7 +1177,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns="" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns="">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -1030,13 +1190,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>6</xdr:col>
+      <xdr:col>7</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>6</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
+      <xdr:col>7</xdr:col>
       <xdr:colOff>12700</xdr:colOff>
       <xdr:row>6</xdr:row>
       <xdr:rowOff>12700</xdr:rowOff>
@@ -1046,7 +1206,7 @@
         <xdr:cNvPr id="10" name="Picture 9" descr="page5image3702672">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BCAE4D06-488E-484E-8B1C-88EBA259AEF7}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns="" id="{BCAE4D06-488E-484E-8B1C-88EBA259AEF7}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1058,7 +1218,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns="" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns="" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -1078,7 +1238,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns="" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns="">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -1091,13 +1251,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>6</xdr:col>
+      <xdr:col>7</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>9</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
+      <xdr:col>7</xdr:col>
       <xdr:colOff>12700</xdr:colOff>
       <xdr:row>9</xdr:row>
       <xdr:rowOff>12700</xdr:rowOff>
@@ -1107,7 +1267,7 @@
         <xdr:cNvPr id="11" name="Picture 10" descr="page5image3703712">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{34A007C2-32FF-F946-A78C-55C38D0F8D6A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns="" id="{34A007C2-32FF-F946-A78C-55C38D0F8D6A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1119,7 +1279,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns="" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns="" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -1139,7 +1299,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns="" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns="">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -1168,7 +1328,7 @@
         <xdr:cNvPr id="12" name="Picture 11" descr="page5image3705792">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A49356F5-0746-F04F-9A08-57C13038F148}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns="" id="{A49356F5-0746-F04F-9A08-57C13038F148}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1180,7 +1340,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns="" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns="" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -1200,7 +1360,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns="" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns="">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -1229,7 +1389,7 @@
         <xdr:cNvPr id="13" name="Picture 12" descr="page5image3706416">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D897A736-EA77-CA45-BE72-EBD7887E488E}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns="" id="{D897A736-EA77-CA45-BE72-EBD7887E488E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1241,7 +1401,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns="" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns="" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -1261,7 +1421,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns="" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns="">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -1290,7 +1450,7 @@
         <xdr:cNvPr id="14" name="Picture 13" descr="page5image3706832">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{336BB3DD-E9B5-F948-AB95-28F2AE85AA33}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns="" id="{336BB3DD-E9B5-F948-AB95-28F2AE85AA33}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1302,7 +1462,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns="" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns="" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -1322,7 +1482,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns="" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns="">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -1351,7 +1511,7 @@
         <xdr:cNvPr id="15" name="Picture 14" descr="page5image3707456">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0C0A9650-BBE9-1248-AFEA-7107D1E31E35}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns="" id="{0C0A9650-BBE9-1248-AFEA-7107D1E31E35}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1363,7 +1523,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns="" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns="" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -1383,7 +1543,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns="" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns="">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -1396,14 +1556,14 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>6</xdr:col>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>800100</xdr:colOff>
       <xdr:row>6</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>61678</xdr:colOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>62711</xdr:colOff>
       <xdr:row>6</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
@@ -1412,7 +1572,7 @@
         <xdr:cNvPr id="16" name="Picture 15" descr="page5image2911024">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{63E28791-EFBD-CB48-8EE3-5E8D0268E1BA}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns="" id="{63E28791-EFBD-CB48-8EE3-5E8D0268E1BA}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1424,7 +1584,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns="" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns="" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -1444,7 +1604,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns="" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns="">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -1457,13 +1617,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>7</xdr:col>
+      <xdr:col>3</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>6</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
+      <xdr:col>3</xdr:col>
       <xdr:colOff>12700</xdr:colOff>
       <xdr:row>6</xdr:row>
       <xdr:rowOff>12700</xdr:rowOff>
@@ -1473,7 +1633,7 @@
         <xdr:cNvPr id="17" name="Picture 16" descr="page5image3706832">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{336BB3DD-E9B5-F948-AB95-28F2AE85AA33}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns="" id="{336BB3DD-E9B5-F948-AB95-28F2AE85AA33}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1485,7 +1645,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns="" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns="" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -1505,7 +1665,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns="" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns="">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -1808,7 +1968,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1819,10 +1979,10 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:L16"/>
+  <dimension ref="A1:N16"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" zoomScale="209" zoomScaleNormal="209" zoomScalePageLayoutView="209" workbookViewId="0">
-      <selection activeCell="M3" sqref="M3"/>
+    <sheetView tabSelected="1" zoomScale="209" zoomScaleNormal="209" zoomScalePageLayoutView="209" workbookViewId="0">
+      <selection activeCell="M9" sqref="M9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1830,40 +1990,42 @@
     <col min="1" max="1" width="11.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="6.83203125" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="7" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.5" style="1" customWidth="1"/>
+    <col min="5" max="5" width="8.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="7" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="6.83203125" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="9.1640625" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="9.5" style="1" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="5.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="18" thickBot="1">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:14" ht="18" thickBot="1">
+      <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>47</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>42</v>
       </c>
       <c r="I1" s="3" t="s">
         <v>3</v>
@@ -1874,34 +2036,37 @@
       <c r="K1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="L1" s="3" t="s">
         <v>6</v>
       </c>
+      <c r="M1" s="18" t="s">
+        <v>71</v>
+      </c>
     </row>
-    <row r="2" spans="1:12" ht="16" customHeight="1">
-      <c r="A2" s="5" t="s">
+    <row r="2" spans="1:14" ht="16" customHeight="1">
+      <c r="A2" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="6">
+      <c r="D2" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="E2" s="6">
         <v>1</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="F2" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="G2" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="H2" s="6" t="s">
         <v>45</v>
-      </c>
-      <c r="H2" s="6" t="s">
-        <v>49</v>
       </c>
       <c r="I2" s="6">
         <v>0</v>
@@ -1912,34 +2077,41 @@
       <c r="K2" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="L2" s="7" t="s">
+      <c r="L2" s="6" t="s">
         <v>45</v>
       </c>
+      <c r="M2" s="19" t="s">
+        <v>76</v>
+      </c>
+      <c r="N2" s="9" t="str">
+        <f>CONCATENATE(E2,F2,G2,H2,I2,J2,K2,L2,M2)</f>
+        <v>101000000000111</v>
+      </c>
     </row>
-    <row r="3" spans="1:12" ht="16" customHeight="1">
-      <c r="A3" s="8" t="s">
+    <row r="3" spans="1:14" ht="16" customHeight="1">
+      <c r="A3" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="9">
+      <c r="B3" s="8">
         <v>100011</v>
       </c>
-      <c r="C3" s="9">
+      <c r="C3" s="10">
         <v>100000</v>
       </c>
-      <c r="D3" s="9">
+      <c r="D3" s="8">
+        <v>100000</v>
+      </c>
+      <c r="E3" s="9">
         <v>1</v>
       </c>
-      <c r="E3" s="9" t="s">
+      <c r="F3" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="F3" s="9" t="s">
+      <c r="G3" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="G3" s="9" t="s">
+      <c r="H3" s="9" t="s">
         <v>51</v>
-      </c>
-      <c r="H3" s="9">
-        <v>100000</v>
       </c>
       <c r="I3" s="9">
         <v>0</v>
@@ -1950,34 +2122,41 @@
       <c r="K3" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="L3" s="10" t="s">
+      <c r="L3" s="9" t="s">
         <v>45</v>
       </c>
+      <c r="M3" s="20" t="s">
+        <v>74</v>
+      </c>
+      <c r="N3" s="9" t="str">
+        <f t="shared" ref="N3:N16" si="0">CONCATENATE(E3,F3,G3,H3,I3,J3,K3,L3,M3)</f>
+        <v>100001000100000</v>
+      </c>
     </row>
-    <row r="4" spans="1:12" ht="16" customHeight="1">
-      <c r="A4" s="8" t="s">
+    <row r="4" spans="1:14" ht="16" customHeight="1">
+      <c r="A4" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="9">
+      <c r="B4" s="8">
         <v>101011</v>
       </c>
-      <c r="C4" s="9">
+      <c r="C4" s="10">
         <v>100000</v>
       </c>
-      <c r="D4" s="9">
+      <c r="D4" s="8">
+        <v>100000</v>
+      </c>
+      <c r="E4" s="9">
         <v>0</v>
       </c>
-      <c r="E4" s="9" t="s">
+      <c r="F4" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="F4" s="9" t="s">
+      <c r="G4" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="G4" s="9" t="s">
+      <c r="H4" s="9" t="s">
         <v>51</v>
-      </c>
-      <c r="H4" s="9">
-        <v>100000</v>
       </c>
       <c r="I4" s="9">
         <v>0</v>
@@ -1988,34 +2167,41 @@
       <c r="K4" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="L4" s="10" t="s">
+      <c r="L4" s="9" t="s">
         <v>45</v>
       </c>
+      <c r="M4" s="20" t="s">
+        <v>74</v>
+      </c>
+      <c r="N4" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>0XX00101XX00000</v>
+      </c>
     </row>
-    <row r="5" spans="1:12" ht="16" customHeight="1">
-      <c r="A5" s="8" t="s">
+    <row r="5" spans="1:14" ht="16" customHeight="1">
+      <c r="A5" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="9" t="s">
+      <c r="B5" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="9">
+      <c r="C5" s="10">
         <v>100010</v>
       </c>
-      <c r="D5" s="9">
+      <c r="D5" s="8">
+        <v>100010</v>
+      </c>
+      <c r="E5" s="9">
         <v>0</v>
       </c>
-      <c r="E5" s="9" t="s">
+      <c r="F5" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="F5" s="9" t="s">
+      <c r="G5" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="G5" s="9" t="s">
+      <c r="H5" s="9" t="s">
         <v>45</v>
-      </c>
-      <c r="H5" s="9">
-        <v>100010</v>
       </c>
       <c r="I5" s="9">
         <v>1</v>
@@ -2026,34 +2212,41 @@
       <c r="K5" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="L5" s="10" t="s">
+      <c r="L5" s="9" t="s">
         <v>45</v>
       </c>
+      <c r="M5" s="20" t="s">
+        <v>75</v>
+      </c>
+      <c r="N5" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>0XX00010XX00001</v>
+      </c>
     </row>
-    <row r="6" spans="1:12" ht="16" customHeight="1">
-      <c r="A6" s="8" t="s">
+    <row r="6" spans="1:14" ht="16" customHeight="1">
+      <c r="A6" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="9" t="s">
+      <c r="B6" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="9" t="s">
+      <c r="C6" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="D6" s="9">
+      <c r="D6" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="E6" s="9">
         <v>0</v>
       </c>
-      <c r="E6" s="9" t="s">
+      <c r="F6" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="F6" s="9" t="s">
+      <c r="G6" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="G6" s="9" t="s">
+      <c r="H6" s="9" t="s">
         <v>53</v>
-      </c>
-      <c r="H6" s="9" t="s">
-        <v>54</v>
       </c>
       <c r="I6" s="9" t="s">
         <v>19</v>
@@ -2064,34 +2257,41 @@
       <c r="K6" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="L6" s="10" t="s">
+      <c r="L6" s="9" t="s">
         <v>51</v>
       </c>
+      <c r="M6" s="20" t="s">
+        <v>74</v>
+      </c>
+      <c r="N6" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>0XXXXXX0XX01000</v>
+      </c>
     </row>
-    <row r="7" spans="1:12" ht="16" customHeight="1" thickBot="1">
-      <c r="A7" s="11" t="s">
+    <row r="7" spans="1:14" ht="16" customHeight="1" thickBot="1">
+      <c r="A7" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="12" t="s">
+      <c r="B7" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="12">
+      <c r="C7" s="13">
         <v>100000</v>
       </c>
-      <c r="D7" s="12">
+      <c r="D7" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="E7" s="12">
         <v>1</v>
       </c>
-      <c r="E7" s="12" t="s">
+      <c r="F7" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="F7" s="12" t="s">
+      <c r="G7" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="G7" s="12" t="s">
+      <c r="H7" s="12" t="s">
         <v>51</v>
-      </c>
-      <c r="H7" s="12" t="s">
-        <v>55</v>
       </c>
       <c r="I7" s="12">
         <v>0</v>
@@ -2102,72 +2302,86 @@
       <c r="K7" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="L7" s="13" t="s">
+      <c r="L7" s="12" t="s">
         <v>45</v>
       </c>
+      <c r="M7" s="21" t="s">
+        <v>74</v>
+      </c>
+      <c r="N7" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>100001000000000</v>
+      </c>
     </row>
-    <row r="8" spans="1:12" ht="16" customHeight="1">
-      <c r="A8" s="5" t="s">
+    <row r="8" spans="1:14" ht="16" customHeight="1">
+      <c r="A8" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="C8" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="D8" s="6" t="s">
+      <c r="D8" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="E8" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="E8" s="6" t="s">
+      <c r="F8" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="F8" s="6" t="s">
+      <c r="G8" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="G8" s="6" t="s">
+      <c r="H8" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="H8" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="I8" s="6" t="s">
+      <c r="I8" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="J8" s="6" t="s">
+      <c r="J8" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="K8" s="6" t="s">
+      <c r="K8" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="L8" s="7" t="s">
+      <c r="L8" s="9" t="s">
         <v>58</v>
       </c>
+      <c r="M8" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="N8" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>0XXXXXX0XX10111</v>
+      </c>
     </row>
-    <row r="9" spans="1:12" ht="16" customHeight="1">
-      <c r="A9" s="8" t="s">
+    <row r="9" spans="1:14" ht="16" customHeight="1">
+      <c r="A9" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="B9" s="9" t="s">
+      <c r="B9" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="C9" s="9" t="s">
+      <c r="C9" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="D9" s="9" t="s">
+      <c r="D9" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="E9" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="E9" s="9" t="s">
+      <c r="F9" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="F9" s="9" t="s">
+      <c r="G9" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="G9" s="9" t="s">
+      <c r="H9" s="9" t="s">
         <v>58</v>
-      </c>
-      <c r="H9" s="9" t="s">
-        <v>60</v>
       </c>
       <c r="I9" s="9" t="s">
         <v>48</v>
@@ -2178,34 +2392,41 @@
       <c r="K9" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="L9" s="10" t="s">
+      <c r="L9" s="9" t="s">
         <v>45</v>
       </c>
+      <c r="M9" s="20" t="s">
+        <v>77</v>
+      </c>
+      <c r="N9" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>100010000000010</v>
+      </c>
     </row>
-    <row r="10" spans="1:12" ht="16" customHeight="1">
-      <c r="A10" s="8" t="s">
+    <row r="10" spans="1:14" ht="16" customHeight="1">
+      <c r="A10" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="B10" s="9" t="s">
+      <c r="B10" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="C10" s="9" t="s">
+      <c r="C10" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="D10" s="9" t="s">
+      <c r="D10" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="E10" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="E10" s="9" t="s">
+      <c r="F10" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="F10" s="9" t="s">
+      <c r="G10" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="G10" s="9" t="s">
+      <c r="H10" s="9" t="s">
         <v>58</v>
-      </c>
-      <c r="H10" s="9" t="s">
-        <v>61</v>
       </c>
       <c r="I10" s="9" t="s">
         <v>48</v>
@@ -2216,34 +2437,41 @@
       <c r="K10" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="L10" s="10" t="s">
+      <c r="L10" s="9" t="s">
         <v>45</v>
       </c>
+      <c r="M10" s="20" t="s">
+        <v>78</v>
+      </c>
+      <c r="N10" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>100010000000011</v>
+      </c>
     </row>
-    <row r="11" spans="1:12" ht="16" customHeight="1">
-      <c r="A11" s="8" t="s">
+    <row r="11" spans="1:14" ht="16" customHeight="1">
+      <c r="A11" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="B11" s="9" t="s">
+      <c r="B11" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="C11" s="9" t="s">
+      <c r="C11" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="D11" s="9" t="s">
+      <c r="D11" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="E11" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="E11" s="9" t="s">
+      <c r="F11" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="F11" s="9" t="s">
+      <c r="G11" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="G11" s="9" t="s">
+      <c r="H11" s="9" t="s">
         <v>53</v>
-      </c>
-      <c r="H11" s="9" t="s">
-        <v>57</v>
       </c>
       <c r="I11" s="9" t="s">
         <v>19</v>
@@ -2254,34 +2482,41 @@
       <c r="K11" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="L11" s="10" t="s">
+      <c r="L11" s="9" t="s">
         <v>51</v>
       </c>
+      <c r="M11" s="20" t="s">
+        <v>72</v>
+      </c>
+      <c r="N11" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>110XXXX01101XXX</v>
+      </c>
     </row>
-    <row r="12" spans="1:12" ht="16" customHeight="1">
-      <c r="A12" s="8" t="s">
+    <row r="12" spans="1:14" ht="16" customHeight="1">
+      <c r="A12" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="B12" s="9" t="s">
+      <c r="B12" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="C12" s="9" t="s">
+      <c r="C12" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="D12" s="9" t="s">
+      <c r="D12" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="E12" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="E12" s="9" t="s">
+      <c r="F12" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="F12" s="9" t="s">
+      <c r="G12" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="G12" s="9" t="s">
+      <c r="H12" s="9" t="s">
         <v>53</v>
-      </c>
-      <c r="H12" s="9" t="s">
-        <v>57</v>
       </c>
       <c r="I12" s="9" t="s">
         <v>48</v>
@@ -2292,34 +2527,41 @@
       <c r="K12" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="L12" s="10" t="s">
+      <c r="L12" s="9" t="s">
         <v>45</v>
       </c>
+      <c r="M12" s="20" t="s">
+        <v>72</v>
+      </c>
+      <c r="N12" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>100XXX001000XXX</v>
+      </c>
     </row>
-    <row r="13" spans="1:12">
-      <c r="A13" s="8" t="s">
+    <row r="13" spans="1:14">
+      <c r="A13" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="B13" s="9" t="s">
+      <c r="B13" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C13" s="9" t="s">
+      <c r="C13" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="D13" s="9" t="s">
+      <c r="D13" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="E13" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="E13" s="9" t="s">
+      <c r="F13" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="F13" s="9" t="s">
+      <c r="G13" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="G13" s="9" t="s">
+      <c r="H13" s="9" t="s">
         <v>45</v>
-      </c>
-      <c r="H13" s="9" t="s">
-        <v>14</v>
       </c>
       <c r="I13" s="9" t="s">
         <v>18</v>
@@ -2330,34 +2572,41 @@
       <c r="K13" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="L13" s="10" t="s">
+      <c r="L13" s="9" t="s">
         <v>63</v>
       </c>
+      <c r="M13" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="N13" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>101X00000000111</v>
+      </c>
     </row>
-    <row r="14" spans="1:12">
-      <c r="A14" s="8" t="s">
+    <row r="14" spans="1:14">
+      <c r="A14" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="B14" s="9" t="s">
+      <c r="B14" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C14" s="9" t="s">
+      <c r="C14" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="D14" s="9" t="s">
+      <c r="D14" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="E14" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="E14" s="9" t="s">
+      <c r="F14" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="F14" s="9" t="s">
+      <c r="G14" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="G14" s="9" t="s">
+      <c r="H14" s="9" t="s">
         <v>70</v>
-      </c>
-      <c r="H14" s="9" t="s">
-        <v>65</v>
       </c>
       <c r="I14" s="9" t="s">
         <v>18</v>
@@ -2368,34 +2617,41 @@
       <c r="K14" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="L14" s="10" t="s">
+      <c r="L14" s="9" t="s">
         <v>45</v>
       </c>
+      <c r="M14" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="N14" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>101000000000111</v>
+      </c>
     </row>
-    <row r="15" spans="1:12">
-      <c r="A15" s="8" t="s">
+    <row r="15" spans="1:14">
+      <c r="A15" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="B15" s="9" t="s">
+      <c r="B15" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C15" s="9" t="s">
+      <c r="C15" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="D15" s="9" t="s">
+      <c r="D15" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="E15" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="E15" s="9" t="s">
+      <c r="F15" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="F15" s="9" t="s">
+      <c r="G15" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="G15" s="9" t="s">
+      <c r="H15" s="9" t="s">
         <v>70</v>
-      </c>
-      <c r="H15" s="9" t="s">
-        <v>66</v>
       </c>
       <c r="I15" s="9" t="s">
         <v>18</v>
@@ -2406,34 +2662,41 @@
       <c r="K15" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="L15" s="10" t="s">
+      <c r="L15" s="9" t="s">
         <v>45</v>
       </c>
+      <c r="M15" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="N15" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>101000000000111</v>
+      </c>
     </row>
-    <row r="16" spans="1:12" ht="16" thickBot="1">
-      <c r="A16" s="11" t="s">
+    <row r="16" spans="1:14" ht="16" thickBot="1">
+      <c r="A16" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="B16" s="12" t="s">
+      <c r="B16" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="C16" s="12" t="s">
+      <c r="C16" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="D16" s="12" t="s">
+      <c r="D16" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="E16" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="E16" s="12" t="s">
+      <c r="F16" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="F16" s="12" t="s">
+      <c r="G16" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="G16" s="12" t="s">
+      <c r="H16" s="12" t="s">
         <v>45</v>
-      </c>
-      <c r="H16" s="12" t="s">
-        <v>55</v>
       </c>
       <c r="I16" s="12" t="s">
         <v>43</v>
@@ -2444,8 +2707,15 @@
       <c r="K16" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="L16" s="13" t="s">
+      <c r="L16" s="12" t="s">
         <v>45</v>
+      </c>
+      <c r="M16" s="21" t="s">
+        <v>73</v>
+      </c>
+      <c r="N16" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>101100000000000</v>
       </c>
     </row>
   </sheetData>
@@ -2455,7 +2725,7 @@
   <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
-      <mx:PLV Mode="1" OnePage="0" WScale="0"/>
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
     </ext>
   </extLst>
 </worksheet>

</xml_diff>

<commit_message>
* updating control, adding factorial.asm
</commit_message>
<xml_diff>
--- a/dessins/Control.xlsx
+++ b/dessins/Control.xlsx
@@ -10,7 +10,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$L$16</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$M$16</definedName>
   </definedNames>
   <calcPr calcId="130407"/>
   <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
@@ -718,7 +718,7 @@
         <xdr:cNvPr id="2" name="Picture 1" descr="page5image5010080">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns="" id="{D1065E6A-2946-EB49-85D5-532CB59FAFF5}"/>
+              <a16:creationId xmlns="" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D1065E6A-2946-EB49-85D5-532CB59FAFF5}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -730,7 +730,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns="" val="0"/>
+              <a14:useLocalDpi xmlns="" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -750,7 +750,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns="">
+            <a14:hiddenFill xmlns="" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -779,7 +779,7 @@
         <xdr:cNvPr id="3" name="Picture 2" descr="page5image5013216">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns="" id="{6B7E070A-7D7D-5E41-A85A-297765A2C47F}"/>
+              <a16:creationId xmlns="" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6B7E070A-7D7D-5E41-A85A-297765A2C47F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -791,7 +791,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns="" val="0"/>
+              <a14:useLocalDpi xmlns="" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -811,7 +811,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns="">
+            <a14:hiddenFill xmlns="" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -840,7 +840,7 @@
         <xdr:cNvPr id="4" name="Picture 3" descr="page5image5027440">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns="" id="{E0BD7523-80DB-9D45-AC23-60E152D26724}"/>
+              <a16:creationId xmlns="" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E0BD7523-80DB-9D45-AC23-60E152D26724}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -852,7 +852,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns="" val="0"/>
+              <a14:useLocalDpi xmlns="" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -872,7 +872,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns="">
+            <a14:hiddenFill xmlns="" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -901,7 +901,7 @@
         <xdr:cNvPr id="5" name="Picture 4" descr="page5image5027664">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns="" id="{3F8DAB48-D435-0543-9727-709FD51CD5FC}"/>
+              <a16:creationId xmlns="" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3F8DAB48-D435-0543-9727-709FD51CD5FC}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -913,7 +913,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns="" val="0"/>
+              <a14:useLocalDpi xmlns="" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -933,7 +933,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns="">
+            <a14:hiddenFill xmlns="" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -962,7 +962,7 @@
         <xdr:cNvPr id="6" name="Picture 5" descr="page5image5027776">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns="" id="{0E82F135-FC04-7E46-A379-6AE6C1F1F79A}"/>
+              <a16:creationId xmlns="" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0E82F135-FC04-7E46-A379-6AE6C1F1F79A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -974,7 +974,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns="" val="0"/>
+              <a14:useLocalDpi xmlns="" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -994,7 +994,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns="">
+            <a14:hiddenFill xmlns="" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -1023,7 +1023,7 @@
         <xdr:cNvPr id="7" name="Picture 6" descr="page5image5051744">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns="" id="{C97A34F3-001F-0F44-9233-FDA963BA405C}"/>
+              <a16:creationId xmlns="" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C97A34F3-001F-0F44-9233-FDA963BA405C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1035,7 +1035,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns="" val="0"/>
+              <a14:useLocalDpi xmlns="" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -1055,7 +1055,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns="">
+            <a14:hiddenFill xmlns="" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -1084,7 +1084,7 @@
         <xdr:cNvPr id="8" name="Picture 7" descr="page5image2911024">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns="" id="{63E28791-EFBD-CB48-8EE3-5E8D0268E1BA}"/>
+              <a16:creationId xmlns="" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{63E28791-EFBD-CB48-8EE3-5E8D0268E1BA}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1096,7 +1096,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns="" val="0"/>
+              <a14:useLocalDpi xmlns="" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -1116,7 +1116,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns="">
+            <a14:hiddenFill xmlns="" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -1145,7 +1145,7 @@
         <xdr:cNvPr id="9" name="Picture 8" descr="page5image3004320">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns="" id="{99CF0BA2-88C3-7942-84F9-F580B832725A}"/>
+              <a16:creationId xmlns="" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{99CF0BA2-88C3-7942-84F9-F580B832725A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1157,7 +1157,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns="" val="0"/>
+              <a14:useLocalDpi xmlns="" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -1177,7 +1177,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns="">
+            <a14:hiddenFill xmlns="" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -1206,7 +1206,7 @@
         <xdr:cNvPr id="10" name="Picture 9" descr="page5image3702672">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns="" id="{BCAE4D06-488E-484E-8B1C-88EBA259AEF7}"/>
+              <a16:creationId xmlns="" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BCAE4D06-488E-484E-8B1C-88EBA259AEF7}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1218,7 +1218,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns="" val="0"/>
+              <a14:useLocalDpi xmlns="" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -1238,7 +1238,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns="">
+            <a14:hiddenFill xmlns="" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -1267,7 +1267,7 @@
         <xdr:cNvPr id="11" name="Picture 10" descr="page5image3703712">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns="" id="{34A007C2-32FF-F946-A78C-55C38D0F8D6A}"/>
+              <a16:creationId xmlns="" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{34A007C2-32FF-F946-A78C-55C38D0F8D6A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1279,7 +1279,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns="" val="0"/>
+              <a14:useLocalDpi xmlns="" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -1299,7 +1299,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns="">
+            <a14:hiddenFill xmlns="" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -1328,7 +1328,7 @@
         <xdr:cNvPr id="12" name="Picture 11" descr="page5image3705792">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns="" id="{A49356F5-0746-F04F-9A08-57C13038F148}"/>
+              <a16:creationId xmlns="" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A49356F5-0746-F04F-9A08-57C13038F148}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1340,7 +1340,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns="" val="0"/>
+              <a14:useLocalDpi xmlns="" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -1360,7 +1360,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns="">
+            <a14:hiddenFill xmlns="" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -1389,7 +1389,7 @@
         <xdr:cNvPr id="13" name="Picture 12" descr="page5image3706416">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns="" id="{D897A736-EA77-CA45-BE72-EBD7887E488E}"/>
+              <a16:creationId xmlns="" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D897A736-EA77-CA45-BE72-EBD7887E488E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1401,7 +1401,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns="" val="0"/>
+              <a14:useLocalDpi xmlns="" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -1421,7 +1421,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns="">
+            <a14:hiddenFill xmlns="" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -1450,7 +1450,7 @@
         <xdr:cNvPr id="14" name="Picture 13" descr="page5image3706832">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns="" id="{336BB3DD-E9B5-F948-AB95-28F2AE85AA33}"/>
+              <a16:creationId xmlns="" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{336BB3DD-E9B5-F948-AB95-28F2AE85AA33}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1462,7 +1462,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns="" val="0"/>
+              <a14:useLocalDpi xmlns="" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -1482,7 +1482,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns="">
+            <a14:hiddenFill xmlns="" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -1511,7 +1511,7 @@
         <xdr:cNvPr id="15" name="Picture 14" descr="page5image3707456">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns="" id="{0C0A9650-BBE9-1248-AFEA-7107D1E31E35}"/>
+              <a16:creationId xmlns="" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0C0A9650-BBE9-1248-AFEA-7107D1E31E35}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1523,7 +1523,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns="" val="0"/>
+              <a14:useLocalDpi xmlns="" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -1543,7 +1543,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns="">
+            <a14:hiddenFill xmlns="" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -1572,7 +1572,7 @@
         <xdr:cNvPr id="16" name="Picture 15" descr="page5image2911024">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns="" id="{63E28791-EFBD-CB48-8EE3-5E8D0268E1BA}"/>
+              <a16:creationId xmlns="" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{63E28791-EFBD-CB48-8EE3-5E8D0268E1BA}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1584,7 +1584,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns="" val="0"/>
+              <a14:useLocalDpi xmlns="" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -1604,7 +1604,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns="">
+            <a14:hiddenFill xmlns="" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -1633,7 +1633,7 @@
         <xdr:cNvPr id="17" name="Picture 16" descr="page5image3706832">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns="" id="{336BB3DD-E9B5-F948-AB95-28F2AE85AA33}"/>
+              <a16:creationId xmlns="" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{336BB3DD-E9B5-F948-AB95-28F2AE85AA33}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1645,7 +1645,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns="" val="0"/>
+              <a14:useLocalDpi xmlns="" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -1665,7 +1665,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns="">
+            <a14:hiddenFill xmlns="" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -1968,7 +1968,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1982,7 +1982,7 @@
   <dimension ref="A1:N16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="209" zoomScaleNormal="209" zoomScalePageLayoutView="209" workbookViewId="0">
-      <selection activeCell="M9" sqref="M9"/>
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1999,7 +1999,7 @@
     <col min="11" max="11" width="9.5" style="1" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="5.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="5.6640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="15" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="18" thickBot="1">

</xml_diff>